<commit_message>
commit change chain data
</commit_message>
<xml_diff>
--- a/Vessels_DATA/CHAIN/MODEL_CHAIN_18800.xlsx
+++ b/Vessels_DATA/CHAIN/MODEL_CHAIN_18800.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evert\Documents\TU-Delft\TIL Master\MT44070 Shipping Management\MT44070_REPO\MT44070_SHIPPING\Vessels_DATA\CHAIN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roeland van Hagen\Documents\Maritieme techniek\Master\MT44070 shipping management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50C20DCD-F759-4B99-99ED-5E43ACC48FC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA059CBE-C2E9-46B7-9F2C-D8DEF100240B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{88B55E88-78A5-4696-84B6-D2825D93A5AB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{56D57881-30F6-4927-8B84-15612AF1F7EC}"/>
   </bookViews>
   <sheets>
     <sheet name="CostChain_TwoNuts" sheetId="1" r:id="rId1"/>
     <sheet name="TimeChain_TwoNuts" sheetId="2" r:id="rId2"/>
     <sheet name="Input data" sheetId="3" r:id="rId3"/>
-    <sheet name="Blad4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1032,7 +1032,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1050,7 +1050,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="nl-NL"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1071,7 +1071,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="nl-NL"/>
+              <a:rPr lang="en-US"/>
               <a:t>Cost built up chain per container (Total chain)</a:t>
             </a:r>
           </a:p>
@@ -1157,7 +1157,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-D05C-4182-8389-FE70999B6202}"/>
+              <c16:uniqueId val="{00000006-6DC3-4FAE-BC01-6DD9E0E969BD}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1232,7 +1232,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000007-D05C-4182-8389-FE70999B6202}"/>
+              <c16:uniqueId val="{00000007-6DC3-4FAE-BC01-6DD9E0E969BD}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1307,7 +1307,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000008-D05C-4182-8389-FE70999B6202}"/>
+              <c16:uniqueId val="{00000008-6DC3-4FAE-BC01-6DD9E0E969BD}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1382,7 +1382,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000009-D05C-4182-8389-FE70999B6202}"/>
+              <c16:uniqueId val="{00000009-6DC3-4FAE-BC01-6DD9E0E969BD}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1457,7 +1457,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000A-D05C-4182-8389-FE70999B6202}"/>
+              <c16:uniqueId val="{0000000A-6DC3-4FAE-BC01-6DD9E0E969BD}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1471,11 +1471,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="169600223"/>
-        <c:axId val="169607903"/>
+        <c:axId val="113230895"/>
+        <c:axId val="113231375"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="169600223"/>
+        <c:axId val="113230895"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1484,7 +1484,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="169607903"/>
+        <c:crossAx val="113231375"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1492,7 +1492,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="169607903"/>
+        <c:axId val="113231375"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1509,7 +1509,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="nl-NL"/>
+                  <a:rPr lang="en-US"/>
                   <a:t>Total chain cost [EUR/container]</a:t>
                 </a:r>
               </a:p>
@@ -1521,7 +1521,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="169600223"/>
+        <c:crossAx val="113230895"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1552,7 +1552,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="nl-NL"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1573,7 +1573,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="nl-NL"/>
+              <a:rPr lang="en-US"/>
               <a:t>Time built up chain per container (Total Time)</a:t>
             </a:r>
           </a:p>
@@ -1659,7 +1659,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-C809-4183-8E44-8C6D96EA021A}"/>
+              <c16:uniqueId val="{00000006-5EC8-44D8-A831-E4F155B26B6A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1734,7 +1734,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000007-C809-4183-8E44-8C6D96EA021A}"/>
+              <c16:uniqueId val="{00000007-5EC8-44D8-A831-E4F155B26B6A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1809,7 +1809,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000008-C809-4183-8E44-8C6D96EA021A}"/>
+              <c16:uniqueId val="{00000008-5EC8-44D8-A831-E4F155B26B6A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1884,7 +1884,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000009-C809-4183-8E44-8C6D96EA021A}"/>
+              <c16:uniqueId val="{00000009-5EC8-44D8-A831-E4F155B26B6A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1959,7 +1959,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000A-C809-4183-8E44-8C6D96EA021A}"/>
+              <c16:uniqueId val="{0000000A-5EC8-44D8-A831-E4F155B26B6A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1973,11 +1973,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="169610783"/>
-        <c:axId val="169598783"/>
+        <c:axId val="113210255"/>
+        <c:axId val="113220335"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="169610783"/>
+        <c:axId val="113210255"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1986,7 +1986,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="169598783"/>
+        <c:crossAx val="113220335"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1994,7 +1994,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="169598783"/>
+        <c:axId val="113220335"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2011,7 +2011,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="nl-NL"/>
+                  <a:rPr lang="en-US"/>
                   <a:t>Total chain time [days]</a:t>
                 </a:r>
               </a:p>
@@ -2023,7 +2023,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="169610783"/>
+        <c:crossAx val="113210255"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2055,23 +2055,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>98425</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2255520</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>142240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>66</xdr:row>
-      <xdr:rowOff>120650</xdr:rowOff>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>71120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Grafiek 1">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55FEF6B8-2E75-8E59-71EC-A467ECA3C017}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E70E4E6-F12E-C33F-B139-D4C3B048AA55}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2097,22 +2097,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>98425</xdr:rowOff>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>66</xdr:row>
-      <xdr:rowOff>120650</xdr:rowOff>
+      <xdr:colOff>327660</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>162560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Grafiek 1">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0F43F95-8242-1561-37AA-1A3C3CF365F8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F91762D8-43C3-9F10-76E3-E1FFD6ABEE4E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2134,7 +2134,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2449,25 +2449,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{460D33CA-9157-43E6-B05E-97C9C5439791}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F35949CD-A685-4929-80BA-110C70C16E8C}">
   <dimension ref="B2:N21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7:N7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="52.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:14" x14ac:dyDescent="0.3">
@@ -3063,25 +3066,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08A69EE6-107D-4813-9749-D630C0913454}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D1B5063-E851-4995-9E63-E289529744CC}">
   <dimension ref="B2:N21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7:N21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="52.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:14" x14ac:dyDescent="0.3">
@@ -3677,33 +3683,37 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{919940B4-C8D5-4350-BA47-515D04CEE4B3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3D32651-7BA7-4C55-9DE6-C91DDAAE595A}">
   <dimension ref="B1:AH119"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="28.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="47.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="40.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="44" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="37.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="37.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="35.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="40" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="22" max="28" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="34" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="36.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="22" max="24" width="8" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="7" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="34" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:34" x14ac:dyDescent="0.3">
@@ -11806,10 +11816,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D316E03C-3E35-49BB-832C-671D78313E09}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92ACC52E-FC88-4362-A18E-009D755DF3B4}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>

</xml_diff>